<commit_message>
Added leaderboard and premium redux store
</commit_message>
<xml_diff>
--- a/Dev log.xlsx
+++ b/Dev log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97ath\OneDrive\Desktop\Full stack apps\Expense tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E57EE1-E055-4976-817F-3EA9413FA708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D999A4-8316-464D-8CF6-8AEB96200FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>#</t>
   </si>
@@ -54,14 +54,100 @@
     <t>const rzp = new window.Razorpay(options); used window.Razorpay() instead of direct import</t>
   </si>
   <si>
-    <t>wrap text in cell: alt+w+h</t>
+    <t>wrap text in cell: alt+h+w</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">By using </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>window.Razorpay</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, you are ensuring that the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>Razorpay</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> object is accessed from the global scope (i.e., the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>window</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> object), rather than from your application's module system. This can be particularly important in cases where the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>Razorpay</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> library has not yet finished loading or has not been properly imported into your application's module system.</t>
+    </r>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Commit ID</t>
+  </si>
+  <si>
+    <t>c99dd7057a6ce50064b27c5f49cced676dfbc442</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +160,11 @@
       <color rgb="FF569CD6"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -96,15 +187,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,53 +484,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="2"/>
     <col min="3" max="3" width="30.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="2"/>
+    <col min="5" max="5" width="21.88671875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="51.77734375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="18.77734375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="21.77734375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="F1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="100.8">
       <c r="A2" s="3">
         <v>45027</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Created custom history component and fixed auth
</commit_message>
<xml_diff>
--- a/Dev log.xlsx
+++ b/Dev log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97ath\OneDrive\Desktop\Full stack apps\Expense tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D999A4-8316-464D-8CF6-8AEB96200FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2764CDC4-6429-4878-95F7-905B562F933A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>#</t>
   </si>
@@ -141,6 +141,21 @@
   </si>
   <si>
     <t>c99dd7057a6ce50064b27c5f49cced676dfbc442</t>
+  </si>
+  <si>
+    <t>front end navigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Front end routing was not working properly. </t>
+  </si>
+  <si>
+    <t>Created a custom history component that can be used outside components and hooks.</t>
+  </si>
+  <si>
+    <t>export const history = {
+    navigate: null,
+    location: null
+}; then initialize this in app like, history.navigate = useNavigate()</t>
   </si>
 </sst>
 </file>
@@ -484,16 +499,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" style="2"/>
     <col min="5" max="5" width="21.88671875" style="4" customWidth="1"/>
@@ -551,6 +566,26 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:8" ht="72">
+      <c r="A3" s="3">
+        <v>45028</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Front end migrated to react
</commit_message>
<xml_diff>
--- a/Dev log.xlsx
+++ b/Dev log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97ath\OneDrive\Desktop\Full stack apps\Expense tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2764CDC4-6429-4878-95F7-905B562F933A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081D0BD0-39EE-4511-B2B6-7F18787E968B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>#</t>
   </si>
@@ -156,6 +156,9 @@
     navigate: null,
     location: null
 }; then initialize this in app like, history.navigate = useNavigate()</t>
+  </si>
+  <si>
+    <t>98cf76e7aedba4e8756074250a5a32de40475c48</t>
   </si>
 </sst>
 </file>
@@ -502,7 +505,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -585,6 +588,9 @@
       <c r="F3" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="G3" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>